<commit_message>
0.6.2 and various little fixes
</commit_message>
<xml_diff>
--- a/shacl-play/src/main/webapp/theme-default/example/PersonCountry.xlsx
+++ b/shacl-play/src/main/webapp/theme-default/example/PersonCountry.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="379">
   <si>
     <t xml:space="preserve">PREFIX</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://d2slcw3kip6qmk.cloudfront.net/marketing/pages/chart/UML-Class-Diagram-Example-Transparent.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doap:repository</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/sparna-git/shacl-play</t>
   </si>
   <si>
     <t xml:space="preserve">This sheet specifies the NodeShape with their targets, that is the sets of entities being validated</t>
@@ -2929,7 +2935,7 @@
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.54"/>
@@ -3168,7 +3174,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -3176,13 +3182,13 @@
       <selection pane="topRight" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.89"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="5" width="27.86"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="42.33"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="26.21"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="26.2"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="48.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="56.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.82"/>
@@ -3305,285 +3311,294 @@
       </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="14"/>
+      <c r="C14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="5"/>
-      <c r="K15" s="15"/>
-    </row>
-    <row r="16" s="16" customFormat="true" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="17" t="s">
+      <c r="A15" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="14"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J16" s="5"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" s="16" customFormat="true" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="D17" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="J16" s="18" t="s">
+      <c r="H17" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="I17" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="L16" s="18" t="s">
+      <c r="J17" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="M16" s="18" t="s">
+      <c r="K17" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="N16" s="18" t="s">
+      <c r="L17" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="O16" s="16" t="s">
+      <c r="M17" s="18" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="44.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="s">
+      <c r="N17" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="O17" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="20" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="44.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="B18" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" s="21" t="s">
+      <c r="E18" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="F18" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="G18" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="H18" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="22" t="s">
+      <c r="I18" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="L17" s="21" t="s">
+      <c r="J18" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="M17" s="21" t="s">
+      <c r="K18" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M18" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="N17" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="O17" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="P17" s="20" t="s">
+      <c r="N18" s="21" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="23" t="s">
+      <c r="O18" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="27"/>
-      <c r="T18" s="27"/>
-    </row>
-    <row r="19" customFormat="false" ht="62.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+      <c r="P18" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="0" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="0" t="str">
-        <f aca="false">CONCATENATE(A19,"-target")</f>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="27"/>
+      <c r="T19" s="27"/>
+    </row>
+    <row r="20" customFormat="false" ht="62.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="0" t="str">
+        <f aca="false">CONCATENATE(A20,"-target")</f>
         <v>sparna:Person-target</v>
       </c>
-      <c r="F19" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="H19" s="0" t="s">
+      <c r="F20" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="H20" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="K19" s="15"/>
-      <c r="M19" s="5" t="s">
+      <c r="I20" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="N19" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="P19" s="0" t="s">
+      <c r="J20" s="5" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="K20" s="15"/>
       <c r="M20" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="N20" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="28"/>
+      <c r="G21" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="N20" s="5" t="n">
+      <c r="H21" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K21" s="15"/>
+      <c r="M21" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="N21" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="P20" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="L22" s="6"/>
-      <c r="M22" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="N22" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="P22" s="0" t="s">
-        <v>104</v>
+      <c r="P21" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>92</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="I23" s="4"/>
       <c r="J23" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L23" s="6"/>
       <c r="M23" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="N23" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="P23" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="N23" s="5" t="n">
+      <c r="B24" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L24" s="6"/>
+      <c r="M24" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N24" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="P23" s="0" t="s">
-        <v>104</v>
+      <c r="P24" s="0" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="https://data.sparna.fr/sparna#"/>
-    <hyperlink ref="D17" r:id="rId2" display="rdfs:comment@en"/>
-    <hyperlink ref="L17" r:id="rId3" display="rdfs:label@fr"/>
-    <hyperlink ref="M17" r:id="rId4" display="rdfs:label@en"/>
-    <hyperlink ref="G19" r:id="rId5" display="http://data.sparna.fr/person/0001"/>
-    <hyperlink ref="I19" r:id="rId6" display="http://data.sparna.fr/person/.$"/>
-    <hyperlink ref="G20" r:id="rId7" display="http://data.sparna.fr/country/France"/>
-    <hyperlink ref="I20" r:id="rId8" display="http://data.sparna.fr/country/.$"/>
-    <hyperlink ref="G22" r:id="rId9" display="http://data.sparna.fr/organization/WS01"/>
-    <hyperlink ref="G23" r:id="rId10" display="http://data.sparna.fr/person/Person_1"/>
+    <hyperlink ref="D18" r:id="rId2" display="rdfs:comment@en"/>
+    <hyperlink ref="L18" r:id="rId3" display="rdfs:label@fr"/>
+    <hyperlink ref="M18" r:id="rId4" display="rdfs:label@en"/>
+    <hyperlink ref="G20" r:id="rId5" display="http://data.sparna.fr/person/0001"/>
+    <hyperlink ref="I20" r:id="rId6" display="http://data.sparna.fr/person/.$"/>
+    <hyperlink ref="G21" r:id="rId7" display="http://data.sparna.fr/country/France"/>
+    <hyperlink ref="I21" r:id="rId8" display="http://data.sparna.fr/country/.$"/>
+    <hyperlink ref="G23" r:id="rId9" display="http://data.sparna.fr/organization/WS01"/>
+    <hyperlink ref="G24" r:id="rId10" display="http://data.sparna.fr/person/Person_1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3608,7 +3623,7 @@
       <selection pane="topRight" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="41.45"/>
@@ -3644,7 +3659,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="11"/>
@@ -3673,83 +3688,83 @@
     </row>
     <row r="5" s="18" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="39" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H5" s="39" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="L5" s="19" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="M5" s="18" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="N5" s="18" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O5" s="18" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="P5" s="18" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="Q5" s="18" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="R5" s="18" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="S5" s="18" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="T5" s="18" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="40" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F6" s="42" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G6" s="43"/>
       <c r="H6" s="43"/>
@@ -3759,72 +3774,72 @@
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="44" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D7" s="46" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F7" s="47" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G7" s="48" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H7" s="48" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I7" s="45" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J7" s="45" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="M7" s="45" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="N7" s="45" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="O7" s="45" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="P7" s="45" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="Q7" s="49" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="R7" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="S7" s="45" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="T7" s="45" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="U7" s="45" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" s="23" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D8" s="50"/>
       <c r="F8" s="51"/>
@@ -3841,16 +3856,16 @@
         <v>sparna:P9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G9" s="30" t="n">
         <v>1</v>
@@ -3859,10 +3874,10 @@
         <v>1</v>
       </c>
       <c r="I9" s="53" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3871,16 +3886,16 @@
         <v>sparna:P10</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G10" s="30" t="n">
         <v>1</v>
@@ -3889,10 +3904,10 @@
         <v>1</v>
       </c>
       <c r="I10" s="53" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3901,13 +3916,13 @@
         <v>sparna:P11</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G11" s="30" t="n">
         <v>1</v>
@@ -3916,10 +3931,10 @@
         <v>1</v>
       </c>
       <c r="I11" s="53" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3928,13 +3943,13 @@
         <v>sparna:P12</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G12" s="30" t="n">
         <v>1</v>
@@ -3944,7 +3959,7 @@
       </c>
       <c r="I12" s="53"/>
       <c r="U12" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3953,16 +3968,16 @@
         <v>sparna:P13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G13" s="30" t="n">
         <v>1</v>
@@ -3971,10 +3986,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="53" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3983,22 +3998,22 @@
         <v>sparna:P14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="I14" s="53" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4007,27 +4022,27 @@
         <v>sparna:P15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G15" s="30" t="n">
         <v>1</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="P15" s="28"/>
       <c r="Q15" s="28"/>
       <c r="T15" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4036,24 +4051,24 @@
         <v>sparna:P16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D16" s="55" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="I16" s="56" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="Q16" s="57" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" s="23" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D17" s="50"/>
       <c r="F17" s="51"/>
@@ -4069,13 +4084,13 @@
         <v>sparna:P18</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G18" s="30" t="n">
         <v>1</v>
@@ -4084,10 +4099,10 @@
         <v>1</v>
       </c>
       <c r="I18" s="56" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="P18" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4096,13 +4111,13 @@
         <v>sparna:P19</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G19" s="30" t="n">
         <v>1</v>
@@ -4111,10 +4126,10 @@
         <v>1</v>
       </c>
       <c r="I19" s="53" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4123,13 +4138,13 @@
         <v>sparna:P20</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G20" s="30" t="n">
         <v>1</v>
@@ -4138,18 +4153,18 @@
         <v>1</v>
       </c>
       <c r="I20" s="53" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" s="64" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="58" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B23" s="58"/>
       <c r="C23" s="58"/>
@@ -4178,24 +4193,24 @@
         <v>sparna:P24</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D24" s="66" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G24" s="67" t="n">
         <v>1</v>
       </c>
       <c r="H24" s="68"/>
       <c r="I24" s="69" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="M24" s="15"/>
       <c r="U24" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4204,13 +4219,13 @@
         <v>sparna:P25</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D25" s="66" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F25" s="57"/>
       <c r="G25" s="67" t="n">
@@ -4218,16 +4233,16 @@
       </c>
       <c r="H25" s="68"/>
       <c r="I25" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="M25" s="15"/>
     </row>
     <row r="26" s="64" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="58" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B26" s="58"/>
       <c r="C26" s="58"/>
@@ -4256,24 +4271,24 @@
         <v>sparna:P27</v>
       </c>
       <c r="B27" s="65" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D27" s="66" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G27" s="67" t="n">
         <v>1</v>
       </c>
       <c r="H27" s="68"/>
       <c r="I27" s="69" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="M27" s="15"/>
       <c r="U27" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4282,13 +4297,13 @@
         <v>sparna:P28</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>43</v>
       </c>
       <c r="D28" s="66" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F28" s="57"/>
       <c r="G28" s="67" t="n">
@@ -4298,10 +4313,10 @@
         <v>1</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J28" s="69" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="M28" s="15"/>
     </row>
@@ -4331,7 +4346,7 @@
       <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.86"/>
@@ -4340,859 +4355,859 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="70" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B1" s="70" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E1" s="70" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="71" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="71" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="72" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E40" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E41" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E42" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E43" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E45" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E46" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E47" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E48" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E49" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E50" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E51" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E52" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E53" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E54" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E55" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E56" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E57" s="0" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E58" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E60" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E61" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E62" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E64" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E65" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E66" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E67" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E68" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E69" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E71" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E72" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E73" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E74" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E75" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E76" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E77" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E78" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E79" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E80" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E81" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E82" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E83" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E84" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E85" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E86" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E87" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E88" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E89" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E90" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E91" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E92" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E93" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E94" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E95" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E96" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E97" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E98" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E99" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E100" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E101" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E102" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E103" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E104" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E105" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E106" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E107" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E108" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E109" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E110" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E111" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E112" s="0" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E113" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E114" s="0" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E115" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E116" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E117" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E118" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E119" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E121" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E122" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E123" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E124" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E125" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E126" s="0" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E127" s="0" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E128" s="0" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E129" s="0" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E130" s="0" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E131" s="0" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E132" s="0" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E133" s="0" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E134" s="0" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E135" s="0" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E136" s="0" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E137" s="0" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E138" s="0" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E139" s="0" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E140" s="0" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E141" s="0" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E142" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E143" s="0" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E144" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E145" s="0" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E146" s="0" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E147" s="0" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E148" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>